<commit_message>
08.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Allocation Sheet.xlsx
+++ b/August/Others/Allocation Sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="111">
   <si>
     <t>BL60</t>
   </si>
@@ -341,10 +341,13 @@
     <t xml:space="preserve">   Total Qnt =</t>
   </si>
   <si>
-    <t>DSR NAME:   Md Robiul Islam</t>
-  </si>
-  <si>
-    <t>Robiul: 01751-312831</t>
+    <t>B65</t>
+  </si>
+  <si>
+    <t>DSR NAME:   Shohel Rana</t>
+  </si>
+  <si>
+    <t>Shohel : 01774-585840</t>
   </si>
 </sst>
 </file>
@@ -763,9 +766,149 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -778,165 +921,25 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1689,1629 +1692,1637 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection sqref="A1:O60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="73"/>
-    <col min="3" max="4" width="8.140625" style="73" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="73" customWidth="1"/>
-    <col min="6" max="6" width="9" style="73" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="73" customWidth="1"/>
-    <col min="8" max="8" width="1.85546875" style="73" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="73" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="73" customWidth="1"/>
-    <col min="11" max="12" width="7.140625" style="73" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="73" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="73" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="73" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="73"/>
+    <col min="1" max="1" width="9.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="44"/>
+    <col min="3" max="4" width="8.140625" style="44" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="44" customWidth="1"/>
+    <col min="6" max="6" width="9" style="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="44" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="44" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="44" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="44" customWidth="1"/>
+    <col min="11" max="12" width="7.140625" style="44" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="44" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="44" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="44" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+    </row>
+    <row r="3" spans="1:15" s="45" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+    </row>
+    <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A4" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="70" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="74" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-    </row>
-    <row r="3" spans="1:15" s="76" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="75" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-    </row>
-    <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="77" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="81" t="s">
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+    </row>
+    <row r="5" spans="1:15" ht="16.5" thickTop="1">
+      <c r="A5" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A6" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="30">
+        <v>800</v>
+      </c>
+      <c r="C6" s="31">
+        <v>875</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="32">
+        <v>6890</v>
+      </c>
+      <c r="K6" s="31">
+        <v>7490</v>
+      </c>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+    </row>
+    <row r="7" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A7" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="30">
+        <v>780</v>
+      </c>
+      <c r="C7" s="31">
+        <v>840</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="34">
+        <v>8340</v>
+      </c>
+      <c r="K7" s="31">
+        <v>8990</v>
+      </c>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+    </row>
+    <row r="8" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A8" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="30">
+        <v>865</v>
+      </c>
+      <c r="C8" s="31">
+        <v>925</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="29">
+        <v>9190</v>
+      </c>
+      <c r="K8" s="31">
+        <v>9990</v>
+      </c>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+    </row>
+    <row r="9" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A9" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="30">
+        <v>810</v>
+      </c>
+      <c r="C9" s="31">
+        <v>880</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="32">
+        <v>5750</v>
+      </c>
+      <c r="K9" s="31">
+        <v>6190</v>
+      </c>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+    </row>
+    <row r="10" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A10" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="30">
+        <v>800</v>
+      </c>
+      <c r="C10" s="31">
+        <v>870</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="32">
+        <v>4280</v>
+      </c>
+      <c r="K10" s="31">
+        <v>4590</v>
+      </c>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+    </row>
+    <row r="11" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A11" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="30">
+        <v>795</v>
+      </c>
+      <c r="C11" s="31">
+        <v>865</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="32">
+        <v>5650</v>
+      </c>
+      <c r="K11" s="31">
+        <v>6150</v>
+      </c>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+    </row>
+    <row r="12" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A12" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="30">
+        <v>790</v>
+      </c>
+      <c r="C12" s="31">
+        <v>860</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="32">
+        <v>5020</v>
+      </c>
+      <c r="K12" s="31">
+        <v>5390</v>
+      </c>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+    </row>
+    <row r="13" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A13" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="30">
+        <v>800</v>
+      </c>
+      <c r="C13" s="31">
+        <v>860</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="32">
+        <v>5280</v>
+      </c>
+      <c r="K13" s="31">
+        <v>5690</v>
+      </c>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+    </row>
+    <row r="14" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A14" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-    </row>
-    <row r="5" spans="1:15" ht="16.5" thickTop="1">
-      <c r="A5" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="44" t="s">
+      <c r="B14" s="30">
+        <v>790</v>
+      </c>
+      <c r="C14" s="31">
+        <v>850</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="32">
+        <v>4550</v>
+      </c>
+      <c r="K14" s="31">
+        <v>4890</v>
+      </c>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+    </row>
+    <row r="15" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A15" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="30">
+        <v>970</v>
+      </c>
+      <c r="C15" s="31">
+        <v>1060</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="32">
+        <v>5100</v>
+      </c>
+      <c r="K15" s="31">
+        <v>5490</v>
+      </c>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+    </row>
+    <row r="16" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A16" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="30">
+        <v>900</v>
+      </c>
+      <c r="C16" s="31">
+        <v>975</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="32">
+        <v>5560</v>
+      </c>
+      <c r="K16" s="31">
+        <v>5990</v>
+      </c>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+    </row>
+    <row r="17" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A17" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="30">
+        <v>915</v>
+      </c>
+      <c r="C17" s="31">
+        <v>990</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="32">
+        <v>6090</v>
+      </c>
+      <c r="K17" s="31">
+        <v>6590</v>
+      </c>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+    </row>
+    <row r="18" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A18" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="30">
+        <v>910</v>
+      </c>
+      <c r="C18" s="31">
+        <v>980</v>
+      </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="32">
+        <v>5390</v>
+      </c>
+      <c r="K18" s="31">
+        <v>5790</v>
+      </c>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+    </row>
+    <row r="19" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A19" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="30">
+        <v>890</v>
+      </c>
+      <c r="C19" s="31">
+        <v>970</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="32">
+        <v>3630</v>
+      </c>
+      <c r="K19" s="31">
+        <v>3890</v>
+      </c>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+    </row>
+    <row r="20" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A20" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="30">
+        <v>920</v>
+      </c>
+      <c r="C20" s="31">
+        <v>999</v>
+      </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="32">
+        <v>3560</v>
+      </c>
+      <c r="K20" s="31">
+        <v>3840</v>
+      </c>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+    </row>
+    <row r="21" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A21" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="30">
+        <v>880</v>
+      </c>
+      <c r="C21" s="31">
+        <v>950</v>
+      </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" s="32">
+        <v>3340</v>
+      </c>
+      <c r="K21" s="31">
+        <v>3590</v>
+      </c>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+    </row>
+    <row r="22" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A22" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="30">
+        <v>845</v>
+      </c>
+      <c r="C22" s="31">
+        <v>910</v>
+      </c>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="32">
+        <v>5390</v>
+      </c>
+      <c r="K22" s="31">
+        <v>5790</v>
+      </c>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+    </row>
+    <row r="23" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A23" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="30">
+        <v>1000</v>
+      </c>
+      <c r="C23" s="31">
+        <v>1090</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="32">
+        <v>4500</v>
+      </c>
+      <c r="K23" s="31">
+        <v>4790</v>
+      </c>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+    </row>
+    <row r="24" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A24" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="30">
+        <v>995</v>
+      </c>
+      <c r="C24" s="31">
+        <v>1075</v>
+      </c>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="32">
+        <v>4970</v>
+      </c>
+      <c r="K24" s="31">
+        <v>5290</v>
+      </c>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+    </row>
+    <row r="25" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A25" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="30">
+        <v>880</v>
+      </c>
+      <c r="C25" s="31">
+        <v>950</v>
+      </c>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="J25" s="32">
+        <v>4015</v>
+      </c>
+      <c r="K25" s="31">
+        <v>4390</v>
+      </c>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+    </row>
+    <row r="26" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A26" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="30">
+        <v>900</v>
+      </c>
+      <c r="C26" s="31">
+        <v>970</v>
+      </c>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="32">
+        <v>3710</v>
+      </c>
+      <c r="K26" s="31">
+        <v>3990</v>
+      </c>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+    </row>
+    <row r="27" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A27" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="30">
+        <v>1040</v>
+      </c>
+      <c r="C27" s="31">
+        <v>1120</v>
+      </c>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="J27" s="32">
+        <v>3620</v>
+      </c>
+      <c r="K27" s="31">
+        <v>3890</v>
+      </c>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+    </row>
+    <row r="28" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A28" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="30">
+        <v>930</v>
+      </c>
+      <c r="C28" s="31">
+        <v>999</v>
+      </c>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="32">
+        <v>4620</v>
+      </c>
+      <c r="K28" s="31">
+        <v>4999</v>
+      </c>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+    </row>
+    <row r="29" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A29" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="30">
+        <v>1290</v>
+      </c>
+      <c r="C29" s="31">
+        <v>1390</v>
+      </c>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="32">
+        <v>4520</v>
+      </c>
+      <c r="K29" s="31">
+        <v>4899</v>
+      </c>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+    </row>
+    <row r="30" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A30" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="30">
+        <v>1190</v>
+      </c>
+      <c r="C30" s="31">
+        <v>1290</v>
+      </c>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30" s="34">
+        <v>4080</v>
+      </c>
+      <c r="K30" s="31">
+        <v>4390</v>
+      </c>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+    </row>
+    <row r="31" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A31" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="30">
+        <v>1270</v>
+      </c>
+      <c r="C31" s="31">
+        <v>1370</v>
+      </c>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="J31" s="34">
+        <v>4220</v>
+      </c>
+      <c r="K31" s="31">
+        <v>4540</v>
+      </c>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
+    </row>
+    <row r="32" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A32" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="30">
+        <v>1170</v>
+      </c>
+      <c r="C32" s="31">
+        <v>1270</v>
+      </c>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="34">
+        <v>12240</v>
+      </c>
+      <c r="K32" s="31">
+        <v>12990</v>
+      </c>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+    </row>
+    <row r="33" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A33" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="30">
+        <v>1190</v>
+      </c>
+      <c r="C33" s="31">
+        <v>1290</v>
+      </c>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="J33" s="32">
+        <v>12090</v>
+      </c>
+      <c r="K33" s="31">
+        <v>12990</v>
+      </c>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="31"/>
+    </row>
+    <row r="34" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A34" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="30">
+        <v>1225</v>
+      </c>
+      <c r="C34" s="31">
+        <v>1325</v>
+      </c>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="J34" s="34">
+        <v>10840</v>
+      </c>
+      <c r="K34" s="31">
+        <v>11990</v>
+      </c>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31"/>
+    </row>
+    <row r="35" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A35" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="30">
+        <v>1220</v>
+      </c>
+      <c r="C35" s="31">
+        <v>1320</v>
+      </c>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="J35" s="32">
+        <v>12490</v>
+      </c>
+      <c r="K35" s="31">
+        <v>13490</v>
+      </c>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+    </row>
+    <row r="36" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A36" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="35">
+        <v>1080</v>
+      </c>
+      <c r="C36" s="31">
+        <v>1160</v>
+      </c>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="J36" s="32">
+        <v>8820</v>
+      </c>
+      <c r="K36" s="31">
+        <v>9490</v>
+      </c>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
+    </row>
+    <row r="37" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A37" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="30">
+        <v>1100</v>
+      </c>
+      <c r="C37" s="31">
+        <v>1199</v>
+      </c>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+    </row>
+    <row r="38" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A38" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="30">
+        <v>1200</v>
+      </c>
+      <c r="C38" s="31">
+        <v>1290</v>
+      </c>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+    </row>
+    <row r="39" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A39" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="30">
+        <v>1010</v>
+      </c>
+      <c r="C39" s="31">
+        <v>1110</v>
+      </c>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+    </row>
+    <row r="40" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A40" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="30">
+        <v>1040</v>
+      </c>
+      <c r="C40" s="31">
+        <v>1130</v>
+      </c>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+    </row>
+    <row r="41" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A41" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="30">
+        <v>1100</v>
+      </c>
+      <c r="C41" s="31">
+        <v>1199</v>
+      </c>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+    </row>
+    <row r="42" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A42" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="30">
+        <v>1100</v>
+      </c>
+      <c r="C42" s="31">
+        <v>1199</v>
+      </c>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+    </row>
+    <row r="43" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A43" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="30">
+        <v>1050</v>
+      </c>
+      <c r="C43" s="31">
+        <v>1130</v>
+      </c>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="31"/>
+    </row>
+    <row r="44" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A44" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="30">
+        <v>1130</v>
+      </c>
+      <c r="C44" s="31">
+        <v>1230</v>
+      </c>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="J44" s="51"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="51"/>
+      <c r="O44" s="36"/>
+    </row>
+    <row r="45" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A45" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="30">
+        <v>1100</v>
+      </c>
+      <c r="C45" s="31">
+        <v>1190</v>
+      </c>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="51"/>
+      <c r="M45" s="51"/>
+      <c r="N45" s="51"/>
+      <c r="O45" s="51"/>
+    </row>
+    <row r="46" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A46" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="30">
+        <v>1330</v>
+      </c>
+      <c r="C46" s="31">
+        <v>1450</v>
+      </c>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="59"/>
+    </row>
+    <row r="47" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A47" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="30">
+        <v>1200</v>
+      </c>
+      <c r="C47" s="31">
+        <v>1299</v>
+      </c>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="J47" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="51"/>
+      <c r="O47" s="60"/>
+    </row>
+    <row r="48" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A48" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="30">
+        <v>1250</v>
+      </c>
+      <c r="C48" s="31">
+        <v>1350</v>
+      </c>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31">
+        <v>1000</v>
+      </c>
+      <c r="J48" s="34"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="31"/>
+      <c r="O48" s="60"/>
+    </row>
+    <row r="49" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A49" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="30">
+        <v>1370</v>
+      </c>
+      <c r="C49" s="31">
+        <v>1490</v>
+      </c>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31">
+        <v>500</v>
+      </c>
+      <c r="J49" s="34"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="60"/>
+    </row>
+    <row r="50" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A50" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="31">
+        <v>2780</v>
+      </c>
+      <c r="C50" s="31">
+        <v>2990</v>
+      </c>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31">
+        <v>100</v>
+      </c>
+      <c r="J50" s="34"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
+      <c r="N50" s="31"/>
+      <c r="O50" s="60"/>
+    </row>
+    <row r="51" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A51" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="31">
+        <v>6540</v>
+      </c>
+      <c r="C51" s="31">
+        <v>6990</v>
+      </c>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="31">
+        <v>50</v>
+      </c>
+      <c r="J51" s="34"/>
+      <c r="K51" s="31"/>
+      <c r="L51" s="31"/>
+      <c r="M51" s="31"/>
+      <c r="N51" s="31"/>
+      <c r="O51" s="60"/>
+    </row>
+    <row r="52" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A52" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="31">
+        <v>5290</v>
+      </c>
+      <c r="C52" s="31">
+        <v>5690</v>
+      </c>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="31">
+        <v>20</v>
+      </c>
+      <c r="J52" s="34"/>
+      <c r="K52" s="31"/>
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
+      <c r="N52" s="31"/>
+      <c r="O52" s="60"/>
+    </row>
+    <row r="53" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A53" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="31">
+        <v>5470</v>
+      </c>
+      <c r="C53" s="31">
+        <v>5890</v>
+      </c>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31">
+        <v>10</v>
+      </c>
+      <c r="J53" s="34"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="31"/>
+      <c r="M53" s="31"/>
+      <c r="N53" s="31"/>
+      <c r="O53" s="60"/>
+    </row>
+    <row r="54" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A54" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="31">
+        <v>5750</v>
+      </c>
+      <c r="C54" s="31">
+        <v>6190</v>
+      </c>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31">
         <v>5</v>
       </c>
-      <c r="F5" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="L5" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="M5" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="N5" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" s="44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A6" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="47">
-        <v>800</v>
-      </c>
-      <c r="C6" s="48">
-        <v>875</v>
-      </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" s="49">
-        <v>8340</v>
-      </c>
-      <c r="K6" s="48">
-        <v>8990</v>
-      </c>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-    </row>
-    <row r="7" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A7" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="47">
-        <v>780</v>
-      </c>
-      <c r="C7" s="48">
-        <v>840</v>
-      </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="51">
-        <v>9190</v>
-      </c>
-      <c r="K7" s="48">
-        <v>9990</v>
-      </c>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
-    </row>
-    <row r="8" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A8" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="47">
-        <v>865</v>
-      </c>
-      <c r="C8" s="48">
-        <v>925</v>
-      </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="46">
-        <v>5750</v>
-      </c>
-      <c r="K8" s="48">
-        <v>6190</v>
-      </c>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-    </row>
-    <row r="9" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A9" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="47">
-        <v>810</v>
-      </c>
-      <c r="C9" s="48">
-        <v>880</v>
-      </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="49">
-        <v>4640</v>
-      </c>
-      <c r="K9" s="48">
-        <v>4990</v>
-      </c>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-    </row>
-    <row r="10" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A10" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="47">
-        <v>800</v>
-      </c>
-      <c r="C10" s="48">
-        <v>870</v>
-      </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="49">
-        <v>5650</v>
-      </c>
-      <c r="K10" s="48">
-        <v>6150</v>
-      </c>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-    </row>
-    <row r="11" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A11" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="47">
-        <v>795</v>
-      </c>
-      <c r="C11" s="48">
-        <v>865</v>
-      </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="49">
-        <v>5020</v>
-      </c>
-      <c r="K11" s="48">
-        <v>5390</v>
-      </c>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-    </row>
-    <row r="12" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A12" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="47">
-        <v>790</v>
-      </c>
-      <c r="C12" s="48">
-        <v>860</v>
-      </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="49">
-        <v>5280</v>
-      </c>
-      <c r="K12" s="48">
-        <v>5690</v>
-      </c>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-    </row>
-    <row r="13" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A13" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="47">
-        <v>800</v>
-      </c>
-      <c r="C13" s="48">
-        <v>860</v>
-      </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="J13" s="49">
-        <v>4820</v>
-      </c>
-      <c r="K13" s="48">
-        <v>5190</v>
-      </c>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-    </row>
-    <row r="14" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A14" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="47">
-        <v>970</v>
-      </c>
-      <c r="C14" s="48">
-        <v>1060</v>
-      </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="49">
-        <v>5100</v>
-      </c>
-      <c r="K14" s="48">
-        <v>5490</v>
-      </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-    </row>
-    <row r="15" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="47">
-        <v>900</v>
-      </c>
-      <c r="C15" s="48">
-        <v>975</v>
-      </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="49">
-        <v>5560</v>
-      </c>
-      <c r="K15" s="48">
-        <v>5990</v>
-      </c>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
-    </row>
-    <row r="16" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A16" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="47">
-        <v>915</v>
-      </c>
-      <c r="C16" s="48">
-        <v>990</v>
-      </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="49">
-        <v>6090</v>
-      </c>
-      <c r="K16" s="48">
-        <v>6590</v>
-      </c>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48"/>
-      <c r="O16" s="48"/>
-    </row>
-    <row r="17" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A17" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="47">
-        <v>910</v>
-      </c>
-      <c r="C17" s="48">
-        <v>980</v>
-      </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="J17" s="49">
-        <v>5390</v>
-      </c>
-      <c r="K17" s="48">
-        <v>5790</v>
-      </c>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
-    </row>
-    <row r="18" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A18" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="47">
-        <v>890</v>
-      </c>
-      <c r="C18" s="48">
-        <v>970</v>
-      </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="J18" s="49">
-        <v>3630</v>
-      </c>
-      <c r="K18" s="48">
-        <v>3890</v>
-      </c>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
-    </row>
-    <row r="19" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A19" s="46" t="s">
+      <c r="J54" s="34"/>
+      <c r="K54" s="31"/>
+      <c r="L54" s="31"/>
+      <c r="M54" s="31"/>
+      <c r="N54" s="31"/>
+      <c r="O54" s="60"/>
+    </row>
+    <row r="55" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A55" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="31">
+        <v>5940</v>
+      </c>
+      <c r="C55" s="31">
+        <v>6390</v>
+      </c>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31">
         <v>2</v>
       </c>
-      <c r="B19" s="47">
-        <v>920</v>
-      </c>
-      <c r="C19" s="48">
-        <v>999</v>
-      </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="49">
-        <v>3560</v>
-      </c>
-      <c r="K19" s="48">
-        <v>3840</v>
-      </c>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="48"/>
-    </row>
-    <row r="20" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A20" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="47">
-        <v>880</v>
-      </c>
-      <c r="C20" s="48">
-        <v>950</v>
-      </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="J20" s="49">
-        <v>3340</v>
-      </c>
-      <c r="K20" s="48">
-        <v>3590</v>
-      </c>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
-    </row>
-    <row r="21" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A21" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="47">
-        <v>845</v>
-      </c>
-      <c r="C21" s="48">
-        <v>910</v>
-      </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="49">
-        <v>5390</v>
-      </c>
-      <c r="K21" s="48">
-        <v>5790</v>
-      </c>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
-    </row>
-    <row r="22" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A22" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="47">
-        <v>1000</v>
-      </c>
-      <c r="C22" s="48">
-        <v>1090</v>
-      </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="J22" s="49">
-        <v>4500</v>
-      </c>
-      <c r="K22" s="48">
-        <v>4790</v>
-      </c>
-      <c r="L22" s="48"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="48"/>
-    </row>
-    <row r="23" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A23" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="47">
-        <v>995</v>
-      </c>
-      <c r="C23" s="48">
-        <v>1075</v>
-      </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" s="49">
-        <v>4970</v>
-      </c>
-      <c r="K23" s="48">
-        <v>5290</v>
-      </c>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
-    </row>
-    <row r="24" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A24" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="47">
-        <v>880</v>
-      </c>
-      <c r="C24" s="48">
-        <v>950</v>
-      </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="J24" s="49">
-        <v>4015</v>
-      </c>
-      <c r="K24" s="48">
-        <v>4390</v>
-      </c>
-      <c r="L24" s="48"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="48"/>
-      <c r="O24" s="48"/>
-    </row>
-    <row r="25" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A25" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="47">
-        <v>960</v>
-      </c>
-      <c r="C25" s="48">
-        <v>1040</v>
-      </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="49">
-        <v>3710</v>
-      </c>
-      <c r="K25" s="48">
-        <v>3990</v>
-      </c>
-      <c r="L25" s="48"/>
-      <c r="M25" s="48"/>
-      <c r="N25" s="48"/>
-      <c r="O25" s="48"/>
-    </row>
-    <row r="26" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A26" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="47">
-        <v>1040</v>
-      </c>
-      <c r="C26" s="48">
-        <v>1120</v>
-      </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="J26" s="49">
-        <v>3620</v>
-      </c>
-      <c r="K26" s="48">
-        <v>3890</v>
-      </c>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
-    </row>
-    <row r="27" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A27" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="47">
-        <v>930</v>
-      </c>
-      <c r="C27" s="48">
-        <v>999</v>
-      </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" s="49">
-        <v>4620</v>
-      </c>
-      <c r="K27" s="48">
-        <v>4999</v>
-      </c>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="48"/>
-    </row>
-    <row r="28" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A28" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" s="47">
-        <v>1290</v>
-      </c>
-      <c r="C28" s="48">
-        <v>1390</v>
-      </c>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="49">
-        <v>4520</v>
-      </c>
-      <c r="K28" s="48">
-        <v>4899</v>
-      </c>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
-      <c r="O28" s="48"/>
-    </row>
-    <row r="29" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A29" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" s="47">
-        <v>1190</v>
-      </c>
-      <c r="C29" s="48">
-        <v>1290</v>
-      </c>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" s="49">
-        <v>4080</v>
-      </c>
-      <c r="K29" s="48">
-        <v>4390</v>
-      </c>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
-      <c r="O29" s="48"/>
-    </row>
-    <row r="30" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A30" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="47">
-        <v>1270</v>
-      </c>
-      <c r="C30" s="48">
-        <v>1370</v>
-      </c>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="J30" s="51">
-        <v>4220</v>
-      </c>
-      <c r="K30" s="48">
-        <v>4540</v>
-      </c>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
-    </row>
-    <row r="31" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A31" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="47">
-        <v>1170</v>
-      </c>
-      <c r="C31" s="48">
-        <v>1270</v>
-      </c>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="50" t="s">
-        <v>55</v>
-      </c>
-      <c r="J31" s="51">
-        <v>12240</v>
-      </c>
-      <c r="K31" s="48">
-        <v>12990</v>
-      </c>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
-      <c r="O31" s="48"/>
-    </row>
-    <row r="32" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A32" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="47">
-        <v>1190</v>
-      </c>
-      <c r="C32" s="48">
-        <v>1290</v>
-      </c>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="J32" s="51">
-        <v>12090</v>
-      </c>
-      <c r="K32" s="48">
-        <v>12990</v>
-      </c>
-      <c r="L32" s="48"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="48"/>
-      <c r="O32" s="48"/>
-    </row>
-    <row r="33" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A33" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="47">
-        <v>1225</v>
-      </c>
-      <c r="C33" s="48">
-        <v>1325</v>
-      </c>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="J33" s="49">
-        <v>10840</v>
-      </c>
-      <c r="K33" s="48">
-        <v>11990</v>
-      </c>
-      <c r="L33" s="48"/>
-      <c r="M33" s="48"/>
-      <c r="N33" s="48"/>
-      <c r="O33" s="48"/>
-    </row>
-    <row r="34" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A34" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="47">
-        <v>1220</v>
-      </c>
-      <c r="C34" s="48">
-        <v>1320</v>
-      </c>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="J34" s="51">
-        <v>12490</v>
-      </c>
-      <c r="K34" s="48">
-        <v>13490</v>
-      </c>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="O34" s="48"/>
-    </row>
-    <row r="35" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A35" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="47">
-        <v>1080</v>
-      </c>
-      <c r="C35" s="48">
-        <v>1160</v>
-      </c>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="J35" s="49">
-        <v>8820</v>
-      </c>
-      <c r="K35" s="48">
-        <v>9490</v>
-      </c>
-      <c r="L35" s="48"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="48"/>
-      <c r="O35" s="48"/>
-    </row>
-    <row r="36" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A36" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="52">
-        <v>1100</v>
-      </c>
-      <c r="C36" s="48">
-        <v>1199</v>
-      </c>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="48"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
-      <c r="O36" s="48"/>
-    </row>
-    <row r="37" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A37" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" s="47">
-        <v>1200</v>
-      </c>
-      <c r="C37" s="48">
-        <v>1290</v>
-      </c>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
-      <c r="M37" s="48"/>
-      <c r="N37" s="48"/>
-      <c r="O37" s="48"/>
-    </row>
-    <row r="38" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A38" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="47">
-        <v>1120</v>
-      </c>
-      <c r="C38" s="48">
-        <v>1220</v>
-      </c>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="48"/>
-      <c r="O38" s="48"/>
-    </row>
-    <row r="39" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A39" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="47">
-        <v>1040</v>
-      </c>
-      <c r="C39" s="48">
-        <v>1130</v>
-      </c>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="48"/>
-      <c r="M39" s="48"/>
-      <c r="N39" s="48"/>
-      <c r="O39" s="48"/>
-    </row>
-    <row r="40" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A40" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="47">
-        <v>1100</v>
-      </c>
-      <c r="C40" s="48">
-        <v>1199</v>
-      </c>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="48"/>
-      <c r="M40" s="48"/>
-      <c r="N40" s="48"/>
-      <c r="O40" s="48"/>
-    </row>
-    <row r="41" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A41" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="47">
-        <v>1100</v>
-      </c>
-      <c r="C41" s="48">
-        <v>1199</v>
-      </c>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="49"/>
-      <c r="K41" s="48"/>
-      <c r="L41" s="48"/>
-      <c r="M41" s="48"/>
-      <c r="N41" s="48"/>
-      <c r="O41" s="48"/>
-    </row>
-    <row r="42" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A42" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="47">
-        <v>1050</v>
-      </c>
-      <c r="C42" s="48">
-        <v>1130</v>
-      </c>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="49"/>
-      <c r="K42" s="48"/>
-      <c r="L42" s="48"/>
-      <c r="M42" s="48"/>
-      <c r="N42" s="48"/>
-      <c r="O42" s="48"/>
-    </row>
-    <row r="43" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A43" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="47">
-        <v>1130</v>
-      </c>
-      <c r="C43" s="48">
-        <v>1230</v>
-      </c>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="49"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="O43" s="48"/>
-    </row>
-    <row r="44" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A44" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="47">
-        <v>1100</v>
-      </c>
-      <c r="C44" s="48">
-        <v>1190</v>
-      </c>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="53" t="s">
+      <c r="J55" s="34"/>
+      <c r="K55" s="31"/>
+      <c r="L55" s="31"/>
+      <c r="M55" s="31"/>
+      <c r="N55" s="31"/>
+      <c r="O55" s="60"/>
+    </row>
+    <row r="56" spans="1:15" ht="17.100000000000001" customHeight="1">
+      <c r="A56" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" s="29">
+        <v>6530</v>
+      </c>
+      <c r="C56" s="29">
+        <v>6990</v>
+      </c>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="53"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="53"/>
-      <c r="N44" s="53"/>
-      <c r="O44" s="54"/>
-    </row>
-    <row r="45" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A45" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="47">
-        <v>1330</v>
-      </c>
-      <c r="C45" s="48">
-        <v>1450</v>
-      </c>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="53"/>
-      <c r="M45" s="53"/>
-      <c r="N45" s="53"/>
-      <c r="O45" s="53"/>
-    </row>
-    <row r="46" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A46" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="47">
-        <v>1200</v>
-      </c>
-      <c r="C46" s="48">
-        <v>1299</v>
-      </c>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="85" t="s">
-        <v>8</v>
-      </c>
-      <c r="J46" s="85"/>
-      <c r="K46" s="85"/>
-      <c r="L46" s="85"/>
-      <c r="M46" s="85"/>
-      <c r="N46" s="85"/>
-      <c r="O46" s="82"/>
-    </row>
-    <row r="47" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A47" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="B47" s="47">
-        <v>1250</v>
-      </c>
-      <c r="C47" s="48">
-        <v>1350</v>
-      </c>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="J47" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="K47" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="L47" s="53"/>
-      <c r="M47" s="53"/>
-      <c r="N47" s="53"/>
-      <c r="O47" s="83"/>
-    </row>
-    <row r="48" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A48" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="47">
-        <v>1370</v>
-      </c>
-      <c r="C48" s="48">
-        <v>1490</v>
-      </c>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="48">
-        <v>1000</v>
-      </c>
-      <c r="J48" s="51"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="48"/>
-      <c r="M48" s="48"/>
-      <c r="N48" s="48"/>
-      <c r="O48" s="83"/>
-    </row>
-    <row r="49" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A49" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="47">
-        <v>2780</v>
-      </c>
-      <c r="C49" s="48">
-        <v>2990</v>
-      </c>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="48">
-        <v>500</v>
-      </c>
-      <c r="J49" s="51"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
-      <c r="M49" s="48"/>
-      <c r="N49" s="48"/>
-      <c r="O49" s="83"/>
-    </row>
-    <row r="50" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A50" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="48">
-        <v>6540</v>
-      </c>
-      <c r="C50" s="48">
-        <v>6990</v>
-      </c>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="48">
-        <v>100</v>
-      </c>
-      <c r="J50" s="51"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="48"/>
-      <c r="M50" s="48"/>
-      <c r="N50" s="48"/>
-      <c r="O50" s="83"/>
-    </row>
-    <row r="51" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A51" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="48">
-        <v>5290</v>
-      </c>
-      <c r="C51" s="48">
-        <v>5690</v>
-      </c>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="48">
-        <v>50</v>
-      </c>
-      <c r="J51" s="51"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="48"/>
-      <c r="M51" s="48"/>
-      <c r="N51" s="48"/>
-      <c r="O51" s="83"/>
-    </row>
-    <row r="52" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A52" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="B52" s="48">
-        <v>5470</v>
-      </c>
-      <c r="C52" s="48">
-        <v>5890</v>
-      </c>
-      <c r="D52" s="48"/>
-      <c r="E52" s="48"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="48"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="48">
-        <v>20</v>
-      </c>
-      <c r="J52" s="51"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="48"/>
-      <c r="M52" s="48"/>
-      <c r="N52" s="48"/>
-      <c r="O52" s="83"/>
-    </row>
-    <row r="53" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A53" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53" s="48">
-        <v>5750</v>
-      </c>
-      <c r="C53" s="48">
-        <v>6190</v>
-      </c>
-      <c r="D53" s="48"/>
-      <c r="E53" s="48"/>
-      <c r="F53" s="48"/>
-      <c r="G53" s="48"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="48">
-        <v>10</v>
-      </c>
-      <c r="J53" s="51"/>
-      <c r="K53" s="48"/>
-      <c r="L53" s="48"/>
-      <c r="M53" s="48"/>
-      <c r="N53" s="48"/>
-      <c r="O53" s="83"/>
-    </row>
-    <row r="54" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A54" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="B54" s="48">
-        <v>5940</v>
-      </c>
-      <c r="C54" s="48">
-        <v>6390</v>
-      </c>
-      <c r="D54" s="48"/>
-      <c r="E54" s="48"/>
-      <c r="F54" s="48"/>
-      <c r="G54" s="48"/>
-      <c r="H54" s="48"/>
-      <c r="I54" s="48">
-        <v>5</v>
-      </c>
-      <c r="J54" s="51"/>
-      <c r="K54" s="48"/>
-      <c r="L54" s="48"/>
-      <c r="M54" s="48"/>
-      <c r="N54" s="48"/>
-      <c r="O54" s="83"/>
-    </row>
-    <row r="55" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A55" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" s="48">
-        <v>6530</v>
-      </c>
-      <c r="C55" s="48">
-        <v>6990</v>
-      </c>
-      <c r="D55" s="48"/>
-      <c r="E55" s="48"/>
-      <c r="F55" s="48"/>
-      <c r="G55" s="48"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="48">
-        <v>2</v>
-      </c>
-      <c r="J55" s="51"/>
-      <c r="K55" s="48"/>
-      <c r="L55" s="48"/>
-      <c r="M55" s="48"/>
-      <c r="N55" s="48"/>
-      <c r="O55" s="83"/>
-    </row>
-    <row r="56" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A56" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" s="46">
-        <v>6890</v>
-      </c>
-      <c r="C56" s="46">
-        <v>7490</v>
-      </c>
-      <c r="D56" s="46"/>
-      <c r="E56" s="46"/>
-      <c r="F56" s="46"/>
-      <c r="G56" s="48"/>
-      <c r="H56" s="48"/>
-      <c r="I56" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="J56" s="48"/>
-      <c r="K56" s="48"/>
-      <c r="L56" s="48"/>
-      <c r="M56" s="48"/>
-      <c r="N56" s="48"/>
-      <c r="O56" s="84"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="31"/>
+      <c r="L56" s="31"/>
+      <c r="M56" s="31"/>
+      <c r="N56" s="31"/>
+      <c r="O56" s="61"/>
     </row>
     <row r="57" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A57" s="55"/>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="55"/>
-      <c r="H57" s="55"/>
-      <c r="I57" s="55"/>
-      <c r="J57" s="66"/>
-      <c r="K57" s="55"/>
-      <c r="L57" s="55"/>
-      <c r="M57" s="67"/>
-      <c r="N57" s="67"/>
-      <c r="O57" s="67"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="40"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
+      <c r="M57" s="41"/>
+      <c r="N57" s="41"/>
+      <c r="O57" s="41"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="64" t="s">
+      <c r="A58" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="64"/>
-      <c r="C58" s="64"/>
-      <c r="D58" s="55"/>
-      <c r="E58" s="55"/>
-      <c r="F58" s="55"/>
-      <c r="G58" s="58" t="s">
+      <c r="B58" s="50"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="H58" s="59"/>
-      <c r="I58" s="60"/>
-      <c r="J58" s="55"/>
-      <c r="K58" s="55"/>
-      <c r="L58" s="55"/>
-      <c r="M58" s="55"/>
-      <c r="N58" s="65" t="s">
+      <c r="H58" s="64"/>
+      <c r="I58" s="65"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
+      <c r="L58" s="37"/>
+      <c r="M58" s="37"/>
+      <c r="N58" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="65"/>
+      <c r="O58" s="62"/>
     </row>
     <row r="59" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A59" s="64"/>
-      <c r="B59" s="64"/>
-      <c r="C59" s="64"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="61"/>
-      <c r="H59" s="62"/>
-      <c r="I59" s="63"/>
-      <c r="J59" s="55"/>
-      <c r="K59" s="55"/>
-      <c r="L59" s="55"/>
-      <c r="M59" s="55"/>
-      <c r="N59" s="64"/>
-      <c r="O59" s="64"/>
+      <c r="A59" s="50"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="66"/>
+      <c r="H59" s="67"/>
+      <c r="I59" s="68"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="37"/>
+      <c r="M59" s="37"/>
+      <c r="N59" s="50"/>
+      <c r="O59" s="50"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="64"/>
-      <c r="B60" s="64"/>
-      <c r="C60" s="64"/>
-      <c r="D60" s="55"/>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="55"/>
-      <c r="H60" s="55"/>
-      <c r="I60" s="55"/>
-      <c r="J60" s="66"/>
-      <c r="K60" s="55"/>
-      <c r="L60" s="55"/>
-      <c r="M60" s="55"/>
-      <c r="N60" s="64"/>
-      <c r="O60" s="64"/>
+      <c r="A60" s="50"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="40"/>
+      <c r="K60" s="37"/>
+      <c r="L60" s="37"/>
+      <c r="M60" s="37"/>
+      <c r="N60" s="50"/>
+      <c r="O60" s="50"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="57"/>
-      <c r="B61" s="57"/>
-      <c r="C61" s="57"/>
-      <c r="D61" s="56"/>
-      <c r="E61" s="56"/>
-      <c r="F61" s="56"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="56"/>
-      <c r="I61" s="56"/>
-      <c r="J61" s="68"/>
-      <c r="K61" s="56"/>
-      <c r="L61" s="56"/>
-      <c r="M61" s="69"/>
-      <c r="N61" s="69"/>
-      <c r="O61" s="69"/>
+      <c r="A61" s="39"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
+      <c r="I61" s="38"/>
+      <c r="J61" s="42"/>
+      <c r="K61" s="38"/>
+      <c r="L61" s="38"/>
+      <c r="M61" s="43"/>
+      <c r="N61" s="43"/>
+      <c r="O61" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="G58:I59"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A1:E1"/>
@@ -3328,8 +3339,6 @@
     <mergeCell ref="O46:O56"/>
     <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="G58:I59"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.3" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3365,73 +3374,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="32" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33" t="s">
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3439,12 +3448,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="37" t="s">
+      <c r="L4" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="6" t="s">
@@ -4548,14 +4557,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="26" t="s">
+      <c r="I44" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="36"/>
+      <c r="J44" s="74"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="26"/>
-      <c r="N44" s="26"/>
+      <c r="M44" s="73"/>
+      <c r="N44" s="73"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -4573,13 +4582,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="26"/>
-      <c r="N45" s="26"/>
-      <c r="O45" s="26"/>
+      <c r="I45" s="73"/>
+      <c r="J45" s="73"/>
+      <c r="K45" s="73"/>
+      <c r="L45" s="73"/>
+      <c r="M45" s="73"/>
+      <c r="N45" s="73"/>
+      <c r="O45" s="73"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="9" t="s">
@@ -4596,15 +4605,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="27" t="s">
+      <c r="I46" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27"/>
-      <c r="O46" s="28"/>
+      <c r="J46" s="75"/>
+      <c r="K46" s="75"/>
+      <c r="L46" s="75"/>
+      <c r="M46" s="75"/>
+      <c r="N46" s="75"/>
+      <c r="O46" s="76"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="9" t="s">
@@ -4627,13 +4636,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="26" t="s">
+      <c r="K47" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="26"/>
-      <c r="M47" s="26"/>
-      <c r="N47" s="26"/>
-      <c r="O47" s="29"/>
+      <c r="L47" s="73"/>
+      <c r="M47" s="73"/>
+      <c r="N47" s="73"/>
+      <c r="O47" s="77"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="9" t="s">
@@ -4658,7 +4667,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="29"/>
+      <c r="O48" s="77"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="9" t="s">
@@ -4683,7 +4692,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="29"/>
+      <c r="O49" s="77"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="4" t="s">
@@ -4708,7 +4717,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="29"/>
+      <c r="O50" s="77"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="4" t="s">
@@ -4733,7 +4742,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="29"/>
+      <c r="O51" s="77"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="4" t="s">
@@ -4758,7 +4767,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="29"/>
+      <c r="O52" s="77"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="4" t="s">
@@ -4783,7 +4792,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="29"/>
+      <c r="O53" s="77"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="4" t="s">
@@ -4808,7 +4817,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="29"/>
+      <c r="O54" s="77"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="4" t="s">
@@ -4833,7 +4842,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="29"/>
+      <c r="O55" s="77"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="9" t="s">
@@ -4858,7 +4867,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="30"/>
+      <c r="O56" s="78"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="17"/>
@@ -4878,49 +4887,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="31" t="s">
+      <c r="A58" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="31"/>
-      <c r="C58" s="31"/>
+      <c r="B58" s="69"/>
+      <c r="C58" s="69"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="42" t="s">
+      <c r="F58" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="42"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="42"/>
-      <c r="J58" s="42"/>
-      <c r="K58" s="42"/>
+      <c r="G58" s="72"/>
+      <c r="H58" s="72"/>
+      <c r="I58" s="72"/>
+      <c r="J58" s="72"/>
+      <c r="K58" s="72"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="41" t="s">
+      <c r="N58" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="41"/>
+      <c r="O58" s="70"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="35"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="35"/>
+      <c r="A59" s="71"/>
+      <c r="B59" s="71"/>
+      <c r="C59" s="71"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="42"/>
-      <c r="H59" s="42"/>
-      <c r="I59" s="42"/>
-      <c r="J59" s="42"/>
-      <c r="K59" s="42"/>
+      <c r="F59" s="72"/>
+      <c r="G59" s="72"/>
+      <c r="H59" s="72"/>
+      <c r="I59" s="72"/>
+      <c r="J59" s="72"/>
+      <c r="K59" s="72"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="35"/>
-      <c r="O59" s="35"/>
+      <c r="N59" s="71"/>
+      <c r="O59" s="71"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="35"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="35"/>
+      <c r="A60" s="71"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="71"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -4931,15 +4940,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="35"/>
-      <c r="O60" s="35"/>
+      <c r="N60" s="71"/>
+      <c r="O60" s="71"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="31"/>
-      <c r="C61" s="31"/>
+      <c r="B61" s="69"/>
+      <c r="C61" s="69"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -4950,11 +4959,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="41"/>
-      <c r="O61" s="41"/>
+      <c r="N61" s="70"/>
+      <c r="O61" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="A59:C60"/>
@@ -4962,19 +4984,6 @@
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="N61:O61"/>
     <mergeCell ref="F58:K59"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
18.08.19 Today sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Allocation Sheet.xlsx
+++ b/August/Others/Allocation Sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="112">
   <si>
     <t>BL60</t>
   </si>
@@ -344,10 +344,13 @@
     <t>B65</t>
   </si>
   <si>
-    <t>DSR NAME:   Shohel Rana</t>
-  </si>
-  <si>
-    <t>Shohel : 01774-585840</t>
+    <t>Offer</t>
+  </si>
+  <si>
+    <t>Robiul: 01751-312831</t>
+  </si>
+  <si>
+    <t>DSR NAME: Md  Robiul Islam</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
       <family val="5"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,6 +515,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -699,7 +708,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -825,6 +834,27 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -870,26 +900,44 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -903,43 +951,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1692,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection sqref="A1:O60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1715,73 +1727,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="47" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="48" t="s">
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
     </row>
     <row r="3" spans="1:15" s="45" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="57"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="64"/>
       <c r="E4" s="46"/>
       <c r="F4" s="46"/>
       <c r="G4" s="46"/>
@@ -1789,12 +1801,12 @@
       <c r="I4" s="46"/>
       <c r="J4" s="46"/>
       <c r="K4" s="46"/>
-      <c r="L4" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
+      <c r="L4" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="26" t="s">
@@ -1828,17 +1840,17 @@
       <c r="K5" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="86" t="s">
+        <v>109</v>
+      </c>
+      <c r="M5" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="27" t="s">
+      <c r="N5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="27" t="s">
+      <c r="O5" s="27" t="s">
         <v>6</v>
-      </c>
-      <c r="O5" s="27" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="17.100000000000001" customHeight="1">
@@ -1894,7 +1906,9 @@
       <c r="K7" s="31">
         <v>8990</v>
       </c>
-      <c r="L7" s="31"/>
+      <c r="L7" s="31">
+        <v>500</v>
+      </c>
       <c r="M7" s="31"/>
       <c r="N7" s="31"/>
       <c r="O7" s="31"/>
@@ -1923,7 +1937,9 @@
       <c r="K8" s="31">
         <v>9990</v>
       </c>
-      <c r="L8" s="31"/>
+      <c r="L8" s="31">
+        <v>1000</v>
+      </c>
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
       <c r="O8" s="31"/>
@@ -2039,7 +2055,9 @@
       <c r="K12" s="31">
         <v>5390</v>
       </c>
-      <c r="L12" s="31"/>
+      <c r="L12" s="31">
+        <v>400</v>
+      </c>
       <c r="M12" s="31"/>
       <c r="N12" s="31"/>
       <c r="O12" s="31"/>
@@ -2126,7 +2144,9 @@
       <c r="K15" s="31">
         <v>5490</v>
       </c>
-      <c r="L15" s="31"/>
+      <c r="L15" s="31">
+        <v>70</v>
+      </c>
       <c r="M15" s="31"/>
       <c r="N15" s="31"/>
       <c r="O15" s="31"/>
@@ -2213,7 +2233,9 @@
       <c r="K18" s="31">
         <v>5790</v>
       </c>
-      <c r="L18" s="31"/>
+      <c r="L18" s="31">
+        <v>200</v>
+      </c>
       <c r="M18" s="31"/>
       <c r="N18" s="31"/>
       <c r="O18" s="31"/>
@@ -2271,7 +2293,9 @@
       <c r="K20" s="31">
         <v>3840</v>
       </c>
-      <c r="L20" s="31"/>
+      <c r="L20" s="31">
+        <v>400</v>
+      </c>
       <c r="M20" s="31"/>
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
@@ -2300,7 +2324,9 @@
       <c r="K21" s="31">
         <v>3590</v>
       </c>
-      <c r="L21" s="31"/>
+      <c r="L21" s="31">
+        <v>320</v>
+      </c>
       <c r="M21" s="31"/>
       <c r="N21" s="31"/>
       <c r="O21" s="31"/>
@@ -2445,7 +2471,9 @@
       <c r="K26" s="31">
         <v>3990</v>
       </c>
-      <c r="L26" s="31"/>
+      <c r="L26" s="31">
+        <v>200</v>
+      </c>
       <c r="M26" s="31"/>
       <c r="N26" s="31"/>
       <c r="O26" s="31"/>
@@ -2474,7 +2502,9 @@
       <c r="K27" s="31">
         <v>3890</v>
       </c>
-      <c r="L27" s="31"/>
+      <c r="L27" s="31">
+        <v>320</v>
+      </c>
       <c r="M27" s="31"/>
       <c r="N27" s="31"/>
       <c r="O27" s="31"/>
@@ -2561,7 +2591,9 @@
       <c r="K30" s="31">
         <v>4390</v>
       </c>
-      <c r="L30" s="31"/>
+      <c r="L30" s="31">
+        <v>200</v>
+      </c>
       <c r="M30" s="31"/>
       <c r="N30" s="31"/>
       <c r="O30" s="31"/>
@@ -2916,14 +2948,14 @@
       <c r="F44" s="31"/>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
-      <c r="I44" s="51" t="s">
+      <c r="I44" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="51"/>
+      <c r="J44" s="58"/>
       <c r="K44" s="31"/>
       <c r="L44" s="31"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="51"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="58"/>
       <c r="O44" s="36"/>
     </row>
     <row r="45" spans="1:15" ht="17.100000000000001" customHeight="1">
@@ -2941,13 +2973,13 @@
       <c r="F45" s="31"/>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
-      <c r="I45" s="51"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="51"/>
-      <c r="L45" s="51"/>
-      <c r="M45" s="51"/>
-      <c r="N45" s="51"/>
-      <c r="O45" s="51"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="58"/>
+      <c r="K45" s="58"/>
+      <c r="L45" s="58"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="58"/>
+      <c r="O45" s="58"/>
     </row>
     <row r="46" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="29" t="s">
@@ -2964,15 +2996,15 @@
       <c r="F46" s="31"/>
       <c r="G46" s="31"/>
       <c r="H46" s="31"/>
-      <c r="I46" s="58" t="s">
+      <c r="I46" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="58"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="58"/>
-      <c r="O46" s="59"/>
+      <c r="J46" s="65"/>
+      <c r="K46" s="65"/>
+      <c r="L46" s="65"/>
+      <c r="M46" s="65"/>
+      <c r="N46" s="65"/>
+      <c r="O46" s="66"/>
     </row>
     <row r="47" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="29" t="s">
@@ -2995,13 +3027,13 @@
       <c r="J47" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="51" t="s">
+      <c r="K47" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="51"/>
-      <c r="M47" s="51"/>
-      <c r="N47" s="51"/>
-      <c r="O47" s="60"/>
+      <c r="L47" s="58"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="58"/>
+      <c r="O47" s="67"/>
     </row>
     <row r="48" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="29" t="s">
@@ -3026,7 +3058,7 @@
       <c r="L48" s="31"/>
       <c r="M48" s="31"/>
       <c r="N48" s="31"/>
-      <c r="O48" s="60"/>
+      <c r="O48" s="67"/>
     </row>
     <row r="49" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="29" t="s">
@@ -3051,7 +3083,7 @@
       <c r="L49" s="31"/>
       <c r="M49" s="31"/>
       <c r="N49" s="31"/>
-      <c r="O49" s="60"/>
+      <c r="O49" s="67"/>
     </row>
     <row r="50" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="31" t="s">
@@ -3076,7 +3108,7 @@
       <c r="L50" s="31"/>
       <c r="M50" s="31"/>
       <c r="N50" s="31"/>
-      <c r="O50" s="60"/>
+      <c r="O50" s="67"/>
     </row>
     <row r="51" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="31" t="s">
@@ -3101,7 +3133,7 @@
       <c r="L51" s="31"/>
       <c r="M51" s="31"/>
       <c r="N51" s="31"/>
-      <c r="O51" s="60"/>
+      <c r="O51" s="67"/>
     </row>
     <row r="52" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="31" t="s">
@@ -3126,7 +3158,7 @@
       <c r="L52" s="31"/>
       <c r="M52" s="31"/>
       <c r="N52" s="31"/>
-      <c r="O52" s="60"/>
+      <c r="O52" s="67"/>
     </row>
     <row r="53" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="31" t="s">
@@ -3151,7 +3183,7 @@
       <c r="L53" s="31"/>
       <c r="M53" s="31"/>
       <c r="N53" s="31"/>
-      <c r="O53" s="60"/>
+      <c r="O53" s="67"/>
     </row>
     <row r="54" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A54" s="31" t="s">
@@ -3176,7 +3208,7 @@
       <c r="L54" s="31"/>
       <c r="M54" s="31"/>
       <c r="N54" s="31"/>
-      <c r="O54" s="60"/>
+      <c r="O54" s="67"/>
     </row>
     <row r="55" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A55" s="31" t="s">
@@ -3201,7 +3233,7 @@
       <c r="L55" s="31"/>
       <c r="M55" s="31"/>
       <c r="N55" s="31"/>
-      <c r="O55" s="60"/>
+      <c r="O55" s="67"/>
     </row>
     <row r="56" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A56" s="29" t="s">
@@ -3226,7 +3258,7 @@
       <c r="L56" s="31"/>
       <c r="M56" s="31"/>
       <c r="N56" s="31"/>
-      <c r="O56" s="61"/>
+      <c r="O56" s="68"/>
     </row>
     <row r="57" spans="1:15" ht="16.5" thickBot="1">
       <c r="A57" s="37"/>
@@ -3246,49 +3278,49 @@
       <c r="O57" s="41"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="50" t="s">
+      <c r="A58" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
       <c r="D58" s="37"/>
       <c r="E58" s="37"/>
       <c r="F58" s="37"/>
-      <c r="G58" s="63" t="s">
+      <c r="G58" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="H58" s="64"/>
-      <c r="I58" s="65"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="50"/>
       <c r="J58" s="37"/>
       <c r="K58" s="37"/>
       <c r="L58" s="37"/>
       <c r="M58" s="37"/>
-      <c r="N58" s="62" t="s">
+      <c r="N58" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="62"/>
+      <c r="O58" s="47"/>
     </row>
     <row r="59" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A59" s="50"/>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
+      <c r="A59" s="57"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
       <c r="D59" s="37"/>
       <c r="E59" s="37"/>
       <c r="F59" s="37"/>
-      <c r="G59" s="66"/>
-      <c r="H59" s="67"/>
-      <c r="I59" s="68"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="53"/>
       <c r="J59" s="37"/>
       <c r="K59" s="37"/>
       <c r="L59" s="37"/>
       <c r="M59" s="37"/>
-      <c r="N59" s="50"/>
-      <c r="O59" s="50"/>
+      <c r="N59" s="57"/>
+      <c r="O59" s="57"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="50"/>
-      <c r="B60" s="50"/>
-      <c r="C60" s="50"/>
+      <c r="A60" s="57"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="57"/>
       <c r="D60" s="37"/>
       <c r="E60" s="37"/>
       <c r="F60" s="37"/>
@@ -3299,8 +3331,8 @@
       <c r="K60" s="37"/>
       <c r="L60" s="37"/>
       <c r="M60" s="37"/>
-      <c r="N60" s="50"/>
-      <c r="O60" s="50"/>
+      <c r="N60" s="57"/>
+      <c r="O60" s="57"/>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" s="39"/>
@@ -3321,6 +3353,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="G58:I59"/>
     <mergeCell ref="F1:J1"/>
@@ -3337,8 +3371,6 @@
     <mergeCell ref="I45:O45"/>
     <mergeCell ref="I46:N46"/>
     <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.3" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3374,73 +3406,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="83" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="81" t="s">
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3448,12 +3480,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="80" t="s">
+      <c r="L4" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="70"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="6" t="s">
@@ -4557,14 +4589,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="73" t="s">
+      <c r="I44" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="74"/>
+      <c r="J44" s="77"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="73"/>
-      <c r="N44" s="73"/>
+      <c r="M44" s="76"/>
+      <c r="N44" s="76"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -4582,13 +4614,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="73"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="73"/>
-      <c r="L45" s="73"/>
-      <c r="M45" s="73"/>
-      <c r="N45" s="73"/>
-      <c r="O45" s="73"/>
+      <c r="I45" s="76"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="76"/>
+      <c r="M45" s="76"/>
+      <c r="N45" s="76"/>
+      <c r="O45" s="76"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="9" t="s">
@@ -4605,15 +4637,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="75" t="s">
+      <c r="I46" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="75"/>
-      <c r="K46" s="75"/>
-      <c r="L46" s="75"/>
-      <c r="M46" s="75"/>
-      <c r="N46" s="75"/>
-      <c r="O46" s="76"/>
+      <c r="J46" s="78"/>
+      <c r="K46" s="78"/>
+      <c r="L46" s="78"/>
+      <c r="M46" s="78"/>
+      <c r="N46" s="78"/>
+      <c r="O46" s="79"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="9" t="s">
@@ -4636,13 +4668,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="73" t="s">
+      <c r="K47" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="73"/>
-      <c r="M47" s="73"/>
-      <c r="N47" s="73"/>
-      <c r="O47" s="77"/>
+      <c r="L47" s="76"/>
+      <c r="M47" s="76"/>
+      <c r="N47" s="76"/>
+      <c r="O47" s="80"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="9" t="s">
@@ -4667,7 +4699,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="77"/>
+      <c r="O48" s="80"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="9" t="s">
@@ -4692,7 +4724,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="77"/>
+      <c r="O49" s="80"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="4" t="s">
@@ -4717,7 +4749,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="77"/>
+      <c r="O50" s="80"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="4" t="s">
@@ -4742,7 +4774,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="77"/>
+      <c r="O51" s="80"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="4" t="s">
@@ -4767,7 +4799,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="77"/>
+      <c r="O52" s="80"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="4" t="s">
@@ -4792,7 +4824,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="77"/>
+      <c r="O53" s="80"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="4" t="s">
@@ -4817,7 +4849,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="77"/>
+      <c r="O54" s="80"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="4" t="s">
@@ -4842,7 +4874,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="77"/>
+      <c r="O55" s="80"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="9" t="s">
@@ -4867,7 +4899,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="78"/>
+      <c r="O56" s="81"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="17"/>
@@ -4887,49 +4919,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="69" t="s">
+      <c r="A58" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="69"/>
-      <c r="C58" s="69"/>
+      <c r="B58" s="82"/>
+      <c r="C58" s="82"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="72" t="s">
+      <c r="F58" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="72"/>
-      <c r="H58" s="72"/>
-      <c r="I58" s="72"/>
-      <c r="J58" s="72"/>
-      <c r="K58" s="72"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="85"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="85"/>
+      <c r="K58" s="85"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="70" t="s">
+      <c r="N58" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="70"/>
+      <c r="O58" s="83"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="71"/>
-      <c r="B59" s="71"/>
-      <c r="C59" s="71"/>
+      <c r="A59" s="84"/>
+      <c r="B59" s="84"/>
+      <c r="C59" s="84"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="72"/>
-      <c r="G59" s="72"/>
-      <c r="H59" s="72"/>
-      <c r="I59" s="72"/>
-      <c r="J59" s="72"/>
-      <c r="K59" s="72"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+      <c r="I59" s="85"/>
+      <c r="J59" s="85"/>
+      <c r="K59" s="85"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="71"/>
-      <c r="O59" s="71"/>
+      <c r="N59" s="84"/>
+      <c r="O59" s="84"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="71"/>
-      <c r="B60" s="71"/>
-      <c r="C60" s="71"/>
+      <c r="A60" s="84"/>
+      <c r="B60" s="84"/>
+      <c r="C60" s="84"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -4940,15 +4972,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="71"/>
-      <c r="O60" s="71"/>
+      <c r="N60" s="84"/>
+      <c r="O60" s="84"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="69" t="s">
+      <c r="A61" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="69"/>
-      <c r="C61" s="69"/>
+      <c r="B61" s="82"/>
+      <c r="C61" s="82"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -4959,11 +4991,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="70"/>
-      <c r="O61" s="70"/>
+      <c r="N61" s="83"/>
+      <c r="O61" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="A59:C60"/>
+    <mergeCell ref="N59:O60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="F58:K59"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A1:E1"/>
@@ -4971,19 +5016,6 @@
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="A59:C60"/>
-    <mergeCell ref="N59:O60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="F58:K59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
29.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Allocation Sheet.xlsx
+++ b/August/Others/Allocation Sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="111">
   <si>
     <t>BL60</t>
   </si>
@@ -347,10 +347,7 @@
     <t>Offer</t>
   </si>
   <si>
-    <t>Robiul: 01751-312831</t>
-  </si>
-  <si>
-    <t>DSR NAME: Md  Robiul Islam</t>
+    <t>DSR NAME: Md  Shohel Rana</t>
   </si>
 </sst>
 </file>
@@ -708,7 +705,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -834,6 +831,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -864,21 +870,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -900,6 +897,36 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -919,39 +946,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1704,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="Q46" sqref="Q46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N59" sqref="A1:O60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1727,65 +1721,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="55" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="54" t="s">
+      <c r="A1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="55" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
     </row>
     <row r="3" spans="1:15" s="45" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
       <c r="A4" s="62" t="s">
@@ -1801,12 +1793,12 @@
       <c r="I4" s="46"/>
       <c r="J4" s="46"/>
       <c r="K4" s="46"/>
-      <c r="L4" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
+      <c r="L4" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="64"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="26" t="s">
@@ -1840,7 +1832,7 @@
       <c r="K5" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="L5" s="86" t="s">
+      <c r="L5" s="47" t="s">
         <v>109</v>
       </c>
       <c r="M5" s="27" t="s">
@@ -2948,14 +2940,14 @@
       <c r="F44" s="31"/>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
-      <c r="I44" s="58" t="s">
+      <c r="I44" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="58"/>
+      <c r="J44" s="48"/>
       <c r="K44" s="31"/>
       <c r="L44" s="31"/>
-      <c r="M44" s="58"/>
-      <c r="N44" s="58"/>
+      <c r="M44" s="48"/>
+      <c r="N44" s="48"/>
       <c r="O44" s="36"/>
     </row>
     <row r="45" spans="1:15" ht="17.100000000000001" customHeight="1">
@@ -2973,13 +2965,13 @@
       <c r="F45" s="31"/>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="58"/>
-      <c r="K45" s="58"/>
-      <c r="L45" s="58"/>
-      <c r="M45" s="58"/>
-      <c r="N45" s="58"/>
-      <c r="O45" s="58"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="48"/>
+      <c r="O45" s="48"/>
     </row>
     <row r="46" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="29" t="s">
@@ -3027,12 +3019,12 @@
       <c r="J47" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="58" t="s">
+      <c r="K47" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="58"/>
-      <c r="M47" s="58"/>
-      <c r="N47" s="58"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="48"/>
       <c r="O47" s="67"/>
     </row>
     <row r="48" spans="1:15" ht="17.100000000000001" customHeight="1">
@@ -3278,49 +3270,49 @@
       <c r="O57" s="41"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="57" t="s">
+      <c r="A58" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="57"/>
-      <c r="C58" s="57"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="49"/>
       <c r="D58" s="37"/>
       <c r="E58" s="37"/>
       <c r="F58" s="37"/>
-      <c r="G58" s="48" t="s">
+      <c r="G58" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="H58" s="49"/>
-      <c r="I58" s="50"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="53"/>
       <c r="J58" s="37"/>
       <c r="K58" s="37"/>
       <c r="L58" s="37"/>
       <c r="M58" s="37"/>
-      <c r="N58" s="47" t="s">
+      <c r="N58" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="47"/>
+      <c r="O58" s="50"/>
     </row>
     <row r="59" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A59" s="57"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="57"/>
+      <c r="A59" s="49"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="49"/>
       <c r="D59" s="37"/>
       <c r="E59" s="37"/>
       <c r="F59" s="37"/>
-      <c r="G59" s="51"/>
-      <c r="H59" s="52"/>
-      <c r="I59" s="53"/>
+      <c r="G59" s="54"/>
+      <c r="H59" s="55"/>
+      <c r="I59" s="56"/>
       <c r="J59" s="37"/>
       <c r="K59" s="37"/>
       <c r="L59" s="37"/>
       <c r="M59" s="37"/>
-      <c r="N59" s="57"/>
-      <c r="O59" s="57"/>
+      <c r="N59" s="49"/>
+      <c r="O59" s="49"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="57"/>
-      <c r="B60" s="57"/>
-      <c r="C60" s="57"/>
+      <c r="A60" s="49"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="49"/>
       <c r="D60" s="37"/>
       <c r="E60" s="37"/>
       <c r="F60" s="37"/>
@@ -3331,8 +3323,8 @@
       <c r="K60" s="37"/>
       <c r="L60" s="37"/>
       <c r="M60" s="37"/>
-      <c r="N60" s="57"/>
-      <c r="O60" s="57"/>
+      <c r="N60" s="49"/>
+      <c r="O60" s="49"/>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" s="39"/>
@@ -3353,6 +3345,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
     <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
@@ -3369,8 +3363,6 @@
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.3" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3406,73 +3398,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="73" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="71" t="s">
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3480,12 +3472,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="70" t="s">
+      <c r="L4" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="6" t="s">
@@ -4589,14 +4581,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="76" t="s">
+      <c r="I44" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="77"/>
+      <c r="J44" s="74"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="76"/>
-      <c r="N44" s="76"/>
+      <c r="M44" s="73"/>
+      <c r="N44" s="73"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -4614,13 +4606,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="76"/>
-      <c r="J45" s="76"/>
-      <c r="K45" s="76"/>
-      <c r="L45" s="76"/>
-      <c r="M45" s="76"/>
-      <c r="N45" s="76"/>
-      <c r="O45" s="76"/>
+      <c r="I45" s="73"/>
+      <c r="J45" s="73"/>
+      <c r="K45" s="73"/>
+      <c r="L45" s="73"/>
+      <c r="M45" s="73"/>
+      <c r="N45" s="73"/>
+      <c r="O45" s="73"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="9" t="s">
@@ -4637,15 +4629,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="78" t="s">
+      <c r="I46" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="78"/>
-      <c r="K46" s="78"/>
-      <c r="L46" s="78"/>
-      <c r="M46" s="78"/>
-      <c r="N46" s="78"/>
-      <c r="O46" s="79"/>
+      <c r="J46" s="75"/>
+      <c r="K46" s="75"/>
+      <c r="L46" s="75"/>
+      <c r="M46" s="75"/>
+      <c r="N46" s="75"/>
+      <c r="O46" s="76"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="9" t="s">
@@ -4668,13 +4660,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="76" t="s">
+      <c r="K47" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="76"/>
-      <c r="M47" s="76"/>
-      <c r="N47" s="76"/>
-      <c r="O47" s="80"/>
+      <c r="L47" s="73"/>
+      <c r="M47" s="73"/>
+      <c r="N47" s="73"/>
+      <c r="O47" s="77"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="9" t="s">
@@ -4699,7 +4691,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="80"/>
+      <c r="O48" s="77"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="9" t="s">
@@ -4724,7 +4716,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="80"/>
+      <c r="O49" s="77"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="4" t="s">
@@ -4749,7 +4741,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="80"/>
+      <c r="O50" s="77"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="4" t="s">
@@ -4774,7 +4766,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="80"/>
+      <c r="O51" s="77"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="4" t="s">
@@ -4799,7 +4791,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="80"/>
+      <c r="O52" s="77"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="4" t="s">
@@ -4824,7 +4816,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="80"/>
+      <c r="O53" s="77"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="4" t="s">
@@ -4849,7 +4841,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="80"/>
+      <c r="O54" s="77"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="4" t="s">
@@ -4874,7 +4866,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="80"/>
+      <c r="O55" s="77"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="9" t="s">
@@ -4899,7 +4891,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="81"/>
+      <c r="O56" s="78"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="17"/>
@@ -4919,49 +4911,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="82" t="s">
+      <c r="A58" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="82"/>
-      <c r="C58" s="82"/>
+      <c r="B58" s="69"/>
+      <c r="C58" s="69"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="85" t="s">
+      <c r="F58" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="85"/>
-      <c r="H58" s="85"/>
-      <c r="I58" s="85"/>
-      <c r="J58" s="85"/>
-      <c r="K58" s="85"/>
+      <c r="G58" s="72"/>
+      <c r="H58" s="72"/>
+      <c r="I58" s="72"/>
+      <c r="J58" s="72"/>
+      <c r="K58" s="72"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="83" t="s">
+      <c r="N58" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="83"/>
+      <c r="O58" s="70"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="84"/>
-      <c r="B59" s="84"/>
-      <c r="C59" s="84"/>
+      <c r="A59" s="71"/>
+      <c r="B59" s="71"/>
+      <c r="C59" s="71"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="85"/>
-      <c r="G59" s="85"/>
-      <c r="H59" s="85"/>
-      <c r="I59" s="85"/>
-      <c r="J59" s="85"/>
-      <c r="K59" s="85"/>
+      <c r="F59" s="72"/>
+      <c r="G59" s="72"/>
+      <c r="H59" s="72"/>
+      <c r="I59" s="72"/>
+      <c r="J59" s="72"/>
+      <c r="K59" s="72"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="84"/>
-      <c r="O59" s="84"/>
+      <c r="N59" s="71"/>
+      <c r="O59" s="71"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="84"/>
-      <c r="B60" s="84"/>
-      <c r="C60" s="84"/>
+      <c r="A60" s="71"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="71"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -4972,15 +4964,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="84"/>
-      <c r="O60" s="84"/>
+      <c r="N60" s="71"/>
+      <c r="O60" s="71"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="82" t="s">
+      <c r="A61" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="82"/>
-      <c r="C61" s="82"/>
+      <c r="B61" s="69"/>
+      <c r="C61" s="69"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -4991,11 +4983,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="83"/>
-      <c r="O61" s="83"/>
+      <c r="N61" s="70"/>
+      <c r="O61" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="A59:C60"/>
@@ -5003,19 +5008,6 @@
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="N61:O61"/>
     <mergeCell ref="F58:K59"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>